<commit_message>
Backup QR Scanner data - 2025-12-04T10:41:21.400Z - Cache Bust: 1764844881400
</commit_message>
<xml_diff>
--- a/log_history/Y3_B2526_Pathology_Lab_Museum_scanner1761032556859_c380f5af5201ef6071e1be103ad2c5029eaceb392a175aad93d8c77cc09c4d35.xlsx
+++ b/log_history/Y3_B2526_Pathology_Lab_Museum_scanner1761032556859_c380f5af5201ef6071e1be103ad2c5029eaceb392a175aad93d8c77cc09c4d35.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Scanner" sheetId="1" r:id="rId1"/>
+    <sheet name="Pathology_Lab_Museum" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -433,338 +433,18 @@
         <v>21/10/2025</v>
       </c>
       <c r="D2" t="str">
-        <v>09:43:04</v>
+        <v>10:43:04</v>
       </c>
       <c r="E2" t="str">
         <v>Manual</v>
       </c>
       <c r="F2" t="str">
-        <v>dalia.t.abdelmegid@med.asu.edu.eg</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>235191</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Pathology Lab/Museum</v>
-      </c>
-      <c r="C3" t="str">
-        <v>21/10/2025</v>
-      </c>
-      <c r="D3" t="str">
-        <v>09:43:21</v>
-      </c>
-      <c r="E3" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F3" t="str">
-        <v>dalia.t.abdelmegid@med.asu.edu.eg</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>234748</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Pathology Lab/Museum</v>
-      </c>
-      <c r="C4" t="str">
-        <v>21/10/2025</v>
-      </c>
-      <c r="D4" t="str">
-        <v>09:43:29</v>
-      </c>
-      <c r="E4" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F4" t="str">
-        <v>dalia.t.abdelmegid@med.asu.edu.eg</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>235010</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Pathology Lab/Museum</v>
-      </c>
-      <c r="C5" t="str">
-        <v>21/10/2025</v>
-      </c>
-      <c r="D5" t="str">
-        <v>09:43:36</v>
-      </c>
-      <c r="E5" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F5" t="str">
-        <v>dalia.t.abdelmegid@med.asu.edu.eg</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>234648</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Pathology Lab/Museum</v>
-      </c>
-      <c r="C6" t="str">
-        <v>21/10/2025</v>
-      </c>
-      <c r="D6" t="str">
-        <v>09:43:46</v>
-      </c>
-      <c r="E6" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F6" t="str">
-        <v>dalia.t.abdelmegid@med.asu.edu.eg</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>235006</v>
-      </c>
-      <c r="B7" t="str">
-        <v>Pathology Lab/Museum</v>
-      </c>
-      <c r="C7" t="str">
-        <v>21/10/2025</v>
-      </c>
-      <c r="D7" t="str">
-        <v>09:43:53</v>
-      </c>
-      <c r="E7" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F7" t="str">
-        <v>dalia.t.abdelmegid@med.asu.edu.eg</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>234628</v>
-      </c>
-      <c r="B8" t="str">
-        <v>Pathology Lab/Museum</v>
-      </c>
-      <c r="C8" t="str">
-        <v>21/10/2025</v>
-      </c>
-      <c r="D8" t="str">
-        <v>09:44:01</v>
-      </c>
-      <c r="E8" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F8" t="str">
-        <v>dalia.t.abdelmegid@med.asu.edu.eg</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>234420</v>
-      </c>
-      <c r="B9" t="str">
-        <v>Pathology Lab/Museum</v>
-      </c>
-      <c r="C9" t="str">
-        <v>21/10/2025</v>
-      </c>
-      <c r="D9" t="str">
-        <v>09:44:08</v>
-      </c>
-      <c r="E9" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F9" t="str">
-        <v>dalia.t.abdelmegid@med.asu.edu.eg</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>234577</v>
-      </c>
-      <c r="B10" t="str">
-        <v>Pathology Lab/Museum</v>
-      </c>
-      <c r="C10" t="str">
-        <v>21/10/2025</v>
-      </c>
-      <c r="D10" t="str">
-        <v>09:44:16</v>
-      </c>
-      <c r="E10" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F10" t="str">
-        <v>dalia.t.abdelmegid@med.asu.edu.eg</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>234572</v>
-      </c>
-      <c r="B11" t="str">
-        <v>Pathology Lab/Museum</v>
-      </c>
-      <c r="C11" t="str">
-        <v>21/10/2025</v>
-      </c>
-      <c r="D11" t="str">
-        <v>09:44:24</v>
-      </c>
-      <c r="E11" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F11" t="str">
-        <v>dalia.t.abdelmegid@med.asu.edu.eg</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="str">
-        <v>235001</v>
-      </c>
-      <c r="B12" t="str">
-        <v>Pathology Lab/Museum</v>
-      </c>
-      <c r="C12" t="str">
-        <v>21/10/2025</v>
-      </c>
-      <c r="D12" t="str">
-        <v>09:44:29</v>
-      </c>
-      <c r="E12" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F12" t="str">
-        <v>dalia.t.abdelmegid@med.asu.edu.eg</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="str">
-        <v>234641</v>
-      </c>
-      <c r="B13" t="str">
-        <v>Pathology Lab/Museum</v>
-      </c>
-      <c r="C13" t="str">
-        <v>21/10/2025</v>
-      </c>
-      <c r="D13" t="str">
-        <v>09:44:37</v>
-      </c>
-      <c r="E13" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F13" t="str">
-        <v>dalia.t.abdelmegid@med.asu.edu.eg</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="str">
-        <v>234929</v>
-      </c>
-      <c r="B14" t="str">
-        <v>Pathology Lab/Museum</v>
-      </c>
-      <c r="C14" t="str">
-        <v>21/10/2025</v>
-      </c>
-      <c r="D14" t="str">
-        <v>09:44:43</v>
-      </c>
-      <c r="E14" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F14" t="str">
-        <v>dalia.t.abdelmegid@med.asu.edu.eg</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="str">
-        <v>235067</v>
-      </c>
-      <c r="B15" t="str">
-        <v>Pathology Lab/Museum</v>
-      </c>
-      <c r="C15" t="str">
-        <v>21/10/2025</v>
-      </c>
-      <c r="D15" t="str">
-        <v>09:45:01</v>
-      </c>
-      <c r="E15" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F15" t="str">
-        <v>dalia.t.abdelmegid@med.asu.edu.eg</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="str">
-        <v>234497</v>
-      </c>
-      <c r="B16" t="str">
-        <v>Pathology Lab/Museum</v>
-      </c>
-      <c r="C16" t="str">
-        <v>21/10/2025</v>
-      </c>
-      <c r="D16" t="str">
-        <v>09:45:08</v>
-      </c>
-      <c r="E16" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F16" t="str">
-        <v>dalia.t.abdelmegid@med.asu.edu.eg</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="str">
-        <v>234963</v>
-      </c>
-      <c r="B17" t="str">
-        <v>Pathology Lab/Museum</v>
-      </c>
-      <c r="C17" t="str">
-        <v>21/10/2025</v>
-      </c>
-      <c r="D17" t="str">
-        <v>09:45:15</v>
-      </c>
-      <c r="E17" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F17" t="str">
-        <v>dalia.t.abdelmegid@med.asu.edu.eg</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="str">
-        <v>234714</v>
-      </c>
-      <c r="B18" t="str">
-        <v>Pathology Lab/Museum</v>
-      </c>
-      <c r="C18" t="str">
-        <v>21/10/2025</v>
-      </c>
-      <c r="D18" t="str">
-        <v>09:45:21</v>
-      </c>
-      <c r="E18" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F18" t="str">
         <v>dalia.t.abdelmegid@med.asu.edu.eg</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F18"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>